<commit_message>
Adatbázis és C# kezdete
C# osztályok létrehozása
C# és Sql összekötése
C#-on belül adat lekérés az adatbázisból
</commit_message>
<xml_diff>
--- a/Documents/Excel_plan.xlsx
+++ b/Documents/Excel_plan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yAn\Documents\GitHub\Aliasly\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yAn\Documents\GitHub\Aliasly-Password-Manager\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D6EBBDC-942E-41CA-A621-104E6CF0A7B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C0FB6D-B783-4AFD-8AAD-8BEC604F7350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{25ED1B67-C117-4AED-9B9D-56E1FC997CAB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{25ED1B67-C117-4AED-9B9D-56E1FC997CAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
   <si>
     <t>Adatbázis</t>
   </si>
@@ -164,15 +164,9 @@
     <t>Adatbázis létrehozás</t>
   </si>
   <si>
-    <t>Adatbázis tervezés</t>
-  </si>
-  <si>
     <t>C# Wpf alap UI</t>
   </si>
   <si>
-    <t>Adatbevitel az Sql adatbázisba C#-al</t>
-  </si>
-  <si>
     <t>Adat titkosítás kivitelezése</t>
   </si>
   <si>
@@ -186,6 +180,12 @@
   </si>
   <si>
     <t>App UI és design</t>
+  </si>
+  <si>
+    <t>C# Osztályok létrehozása</t>
+  </si>
+  <si>
+    <t>Adat írás/olvasás az Sql adatbázisba C#-al</t>
   </si>
 </sst>
 </file>
@@ -216,7 +216,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -243,19 +243,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -272,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -281,12 +275,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -626,49 +619,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2DC08AE-91D2-4E7D-A50D-256CD96B77DD}">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="6"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="7"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -678,11 +669,8 @@
       <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -695,10 +683,8 @@
       <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
@@ -714,17 +700,8 @@
       <c r="E5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="6"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -737,18 +714,8 @@
       <c r="D7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
@@ -758,25 +725,17 @@
       <c r="C9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F11" s="6"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C10" s="6"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>24</v>
       </c>
@@ -790,98 +749,90 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="9" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B13" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="9" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B14" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="9" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B15" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="9" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C16" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="10" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="9" t="s">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C17" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="6"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="9" t="s">
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C18" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="6"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" s="5" t="s">
+      <c r="F20" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H20" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="I20" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F20" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G20" s="5" t="s">
+      <c r="J20" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K20" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="J20" s="5" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adatbázis kezelés és kisebb dolgok
</commit_message>
<xml_diff>
--- a/Documents/Excel_plan.xlsx
+++ b/Documents/Excel_plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yAn\Documents\GitHub\Aliasly-Password-Manager\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7DC9E90-8395-46EB-B50E-48164AAE8A49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164B376F-06F9-4152-BA79-73258F1B0EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{25ED1B67-C117-4AED-9B9D-56E1FC997CAB}"/>
   </bookViews>
@@ -663,7 +663,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -716,7 +716,7 @@
       <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="8" t="s">
         <v>42</v>
       </c>
     </row>
@@ -727,7 +727,7 @@
       <c r="B4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="10" t="s">
@@ -749,7 +749,7 @@
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="8" t="s">
         <v>44</v>
       </c>
     </row>
@@ -762,7 +762,7 @@
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="10" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -790,7 +790,7 @@
       <c r="C9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="13" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Megjelenítés javítása + egyeb dolgok
</commit_message>
<xml_diff>
--- a/Documents/Excel_plan.xlsx
+++ b/Documents/Excel_plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yAn\Documents\GitHub\Aliasly-Password-Manager\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164B376F-06F9-4152-BA79-73258F1B0EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D78FF23-2C32-41B8-8F3F-E53A2833F892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{25ED1B67-C117-4AED-9B9D-56E1FC997CAB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
   <si>
     <t>Adatbázis</t>
   </si>
@@ -83,9 +83,6 @@
     <t>AES-256</t>
   </si>
   <si>
-    <t>PBKDF2</t>
-  </si>
-  <si>
     <t>Mester kulcs</t>
   </si>
   <si>
@@ -95,9 +92,6 @@
     <t>Jelszó generálás</t>
   </si>
   <si>
-    <t>Salting</t>
-  </si>
-  <si>
     <t>Sql táblák</t>
   </si>
   <si>
@@ -113,21 +107,12 @@
     <t>url</t>
   </si>
   <si>
-    <t>hozzáfűzés</t>
-  </si>
-  <si>
     <t>log_id</t>
   </si>
   <si>
     <t>Hozzáférés log</t>
   </si>
   <si>
-    <t>leírás</t>
-  </si>
-  <si>
-    <t>dátum idő</t>
-  </si>
-  <si>
     <t>Roadmap</t>
   </si>
   <si>
@@ -137,9 +122,6 @@
     <t>C# Wpf alap UI</t>
   </si>
   <si>
-    <t>Adat titkosítás kivitelezése</t>
-  </si>
-  <si>
     <t>Extrák</t>
   </si>
   <si>
@@ -155,9 +137,6 @@
     <t>C# Osztályok létrehozása</t>
   </si>
   <si>
-    <t>Adat írás/olvasás az Sql adatbázisba C#-al</t>
-  </si>
-  <si>
     <t>Metódusok</t>
   </si>
   <si>
@@ -182,18 +161,9 @@
     <t>Jelszó és felhasználó tárolás</t>
   </si>
   <si>
-    <t>Hashing metódus</t>
-  </si>
-  <si>
     <t>Encryption metódus</t>
   </si>
   <si>
-    <t>hashed_kulcs</t>
-  </si>
-  <si>
-    <t>salt_string</t>
-  </si>
-  <si>
     <t>jelszo_id</t>
   </si>
   <si>
@@ -215,7 +185,31 @@
     <t>titkositas</t>
   </si>
   <si>
-    <t>Hashing</t>
+    <t>encrypted_kulcs</t>
+  </si>
+  <si>
+    <t>datum_ido</t>
+  </si>
+  <si>
+    <t>leiras</t>
+  </si>
+  <si>
+    <t>hozzafuzes</t>
+  </si>
+  <si>
+    <t>Jelszó erősség ellenőrzés</t>
+  </si>
+  <si>
+    <t>Backup File generálás</t>
+  </si>
+  <si>
+    <t>Adattitkosítás kivitelezése</t>
+  </si>
+  <si>
+    <t>Adatírás/olvasás az Sql adatbázisba C#-al</t>
+  </si>
+  <si>
+    <t>Adattitkosítás</t>
   </si>
 </sst>
 </file>
@@ -663,7 +657,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -694,7 +688,7 @@
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
       <c r="G1" s="12" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -703,7 +697,7 @@
       <c r="C2" s="6"/>
       <c r="D2" s="7"/>
       <c r="G2" s="8" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -717,7 +711,7 @@
         <v>8</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -731,31 +725,35 @@
         <v>9</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>6</v>
+        <v>57</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
+      <c r="D5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="G5" s="8" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G6" s="5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -772,156 +770,142 @@
         <v>12</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G8" s="13" t="s">
-        <v>48</v>
+      <c r="G8" s="8" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B9" s="10" t="s">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="6"/>
+      <c r="C11" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>27</v>
+      <c r="B12" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B13" s="11" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B14" s="11" t="s">
+      <c r="C14" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" s="11" t="s">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C15" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B15" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>21</v>
-      </c>
       <c r="E15" s="11" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C16" s="11" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C17" s="11" t="s">
-        <v>23</v>
-      </c>
       <c r="D17" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D18" s="11" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="E20" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="I20" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G20" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="H20" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>37</v>
       </c>
       <c r="J20" s="5" t="s">
         <v>10</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>